<commit_message>
pages/tests edited and headless mode integrated
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aditikhulbe\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACAE4E4-5ADF-4CF7-9AC6-D79C89FA3E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62994EC1-B1E1-4F3C-A63B-9EB6E23A0DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="AgentLogin" sheetId="3" r:id="rId2"/>
-    <sheet name="Ticket" sheetId="4" r:id="rId3"/>
-    <sheet name="Blog" sheetId="5" r:id="rId4"/>
-    <sheet name="MobilePage" sheetId="6" r:id="rId5"/>
-    <sheet name="SMSlinkPage" sheetId="7" r:id="rId6"/>
+    <sheet name="Ticket" sheetId="4" r:id="rId2"/>
+    <sheet name="Blog" sheetId="5" r:id="rId3"/>
+    <sheet name="MobilePage" sheetId="6" r:id="rId4"/>
+    <sheet name="SMSlinkPage" sheetId="7" r:id="rId5"/>
+    <sheet name="BusHirePage" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,13 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>TicketNo</t>
   </si>
@@ -59,12 +53,6 @@
     <t>aditi@gmail.com</t>
   </si>
   <si>
-    <t>AgentWantstoLogin</t>
-  </si>
-  <si>
-    <t>aditikhulbe</t>
-  </si>
-  <si>
     <t>BlogSearch</t>
   </si>
   <si>
@@ -105,6 +93,39 @@
   </si>
   <si>
     <t>7428532513</t>
+  </si>
+  <si>
+    <t>whenUserEntersValidInformationForOutstation</t>
+  </si>
+  <si>
+    <t>Pickup Location</t>
+  </si>
+  <si>
+    <t>Destination Location</t>
+  </si>
+  <si>
+    <t>Number of Passengers</t>
+  </si>
+  <si>
+    <t>From Date and Time</t>
+  </si>
+  <si>
+    <t>Till Date and Time</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>New Delhi Metro Station</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>4-07-2021-10:20 AM</t>
+  </si>
+  <si>
+    <t>5-07-2021-11:00 AM</t>
   </si>
 </sst>
 </file>
@@ -148,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -162,6 +183,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,24 +491,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -488,66 +521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F625CB-BA2B-46BC-ADEF-CDAAF0618FFE}">
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="J14" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2536051-9700-4106-8A08-EE7B9B7F9782}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,30 +538,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -599,12 +577,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2729CD08-348C-4631-9DD8-60E039600406}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,25 +595,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -644,7 +622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92331BFB-4E94-469E-8344-721D1BBA0860}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -661,24 +639,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -686,11 +664,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15CA679-64BF-41AB-904B-E47E5CA49BE4}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -704,30 +682,104 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72FA836-B258-4038-93DF-0FC0B18462AC}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" customWidth="1"/>
+    <col min="7" max="7" width="18.90625" customWidth="1"/>
+    <col min="8" max="8" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added jenkins doc file
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aditikhulbe\Desktop\work space\FinalAssignment\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE033AE4-B010-4E8C-B52B-1A9063492229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEF69C1-0654-4190-BD30-A21F59CA5B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Blog" sheetId="5" r:id="rId3"/>
     <sheet name="MobilePage" sheetId="6" r:id="rId4"/>
     <sheet name="SMSlinkPage" sheetId="7" r:id="rId5"/>
-    <sheet name="BusHirePage" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>TicketNo</t>
   </si>
@@ -93,39 +92,6 @@
   </si>
   <si>
     <t>7428532513</t>
-  </si>
-  <si>
-    <t>whenUserEntersValidInformationForOutstation</t>
-  </si>
-  <si>
-    <t>Pickup Location</t>
-  </si>
-  <si>
-    <t>Destination Location</t>
-  </si>
-  <si>
-    <t>Number of Passengers</t>
-  </si>
-  <si>
-    <t>From Date and Time</t>
-  </si>
-  <si>
-    <t>Till Date and Time</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>New Delhi Metro Station</t>
-  </si>
-  <si>
-    <t>Noida</t>
-  </si>
-  <si>
-    <t>20-07-2021-10:20 AM</t>
-  </si>
-  <si>
-    <t>22-07-2021-11:00 AM</t>
   </si>
 </sst>
 </file>
@@ -169,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,21 +149,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,7 +536,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -714,78 +665,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72FA836-B258-4038-93DF-0FC0B18462AC}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" customWidth="1"/>
-    <col min="7" max="7" width="18.90625" customWidth="1"/>
-    <col min="8" max="8" width="14.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="9">
-        <v>12</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>